<commit_message>
Update resultados - 2026-02-13 23:02:36
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,24 +573,24 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Albatros</t>
+          <t>Principiantes</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>damas</t>
+          <t>general</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Ferrante Keller, María Estefanía</t>
+          <t>Bogado, Ogán</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7">
@@ -601,7 +601,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Prejuveniles</t>
+          <t>Albatros</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -634,7 +634,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>caballeros</t>
+          <t>damas</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -642,10 +642,38 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
+          <t>Ferrante Keller, María Estefanía</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Torneo FEG</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Prejuveniles</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>caballeros</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>Petric, Juan Cruz</t>
         </is>
       </c>
-      <c r="F8" t="n">
+      <c r="F9" t="n">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update resultados - 2026-02-13 23:15:59
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -601,24 +601,24 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Albatros</t>
+          <t>Principiantes</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>damas</t>
+          <t>general</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Ferrante Keller, María Estefanía</t>
+          <t>Vera, Bautista</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>93</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
@@ -629,7 +629,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Prejuveniles</t>
+          <t>Albatros</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -662,7 +662,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>caballeros</t>
+          <t>damas</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -670,10 +670,38 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
+          <t>Ferrante Keller, María Estefanía</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Torneo FEG</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Prejuveniles</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>caballeros</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
           <t>Petric, Juan Cruz</t>
         </is>
       </c>
-      <c r="F9" t="n">
+      <c r="F10" t="n">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update resultados - 2026-02-13 23:56:10
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -629,24 +629,24 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Albatros</t>
+          <t>Principiantes</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>damas</t>
+          <t>general</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Ferrante Keller, María Estefanía</t>
+          <t>Esborraz, Juan Cruz</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>93</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9">
@@ -657,24 +657,24 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Prejuveniles</t>
+          <t>Principiantes</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>damas</t>
+          <t>general</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Ferrante Keller, María Estefanía</t>
+          <t>Núñez, Valentino</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>93</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10">
@@ -685,12 +685,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Prejuveniles</t>
+          <t>Albatros</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>caballeros</t>
+          <t>damas</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -698,11 +698,95 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
+          <t>Ferrante Keller, María Estefanía</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Torneo FEG</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Prejuveniles</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>damas</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Ferrante Keller, María Estefanía</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Torneo FEG</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Prejuveniles</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>caballeros</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
           <t>Petric, Juan Cruz</t>
         </is>
       </c>
-      <c r="F10" t="n">
+      <c r="F12" t="n">
         <v>86</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Torneo FEG</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Juveniles</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>caballeros</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Liberatori, Augusto</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update resultados - 2026-02-14 00:00:10
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -713,12 +713,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Prejuveniles</t>
+          <t>Albatros</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>damas</t>
+          <t>caballeros</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -726,11 +726,11 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Ferrante Keller, María Estefanía</t>
+          <t>Montoto, Manuel</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>93</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12">
@@ -746,7 +746,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>caballeros</t>
+          <t>damas</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -754,11 +754,11 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Petric, Juan Cruz</t>
+          <t>Ferrante Keller, María Estefanía</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>86</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13">
@@ -769,7 +769,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Juveniles</t>
+          <t>Prejuveniles</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -782,11 +782,67 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
+          <t>Petric, Juan Cruz</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Torneo FEG</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Juveniles</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>caballeros</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>1</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
           <t>Liberatori, Augusto</t>
         </is>
       </c>
-      <c r="F13" t="n">
+      <c r="F14" t="n">
         <v>75</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Torneo FEG</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Juveniles</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>caballeros</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Porzio, Tomás</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update resultados - 2026-02-14 01:09:33
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,6 +452,11 @@
           <t>total</t>
         </is>
       </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>estado</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -480,6 +485,11 @@
       <c r="F2" t="n">
         <v>19</v>
       </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -502,11 +512,16 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Luján Martínez, Benjamín</t>
+          <t>Micheloud, Artemio</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -530,11 +545,16 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Micheloud, Artemio</t>
+          <t>Elcura, Lorenzo</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -558,11 +578,16 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Elcura, Lorenzo</t>
+          <t>Bogado, Ogán</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>23</v>
+        <v>33</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -586,11 +611,16 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Bogado, Ogán</t>
+          <t>Vera, Bautista</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -614,11 +644,16 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Vera, Bautista</t>
+          <t>Esborraz, Juan Cruz</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>34</v>
+        <v>38</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -642,11 +677,16 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Esborraz, Juan Cruz</t>
+          <t>Núñez, Valentino</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -657,24 +697,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Principiantes</t>
+          <t>Birdies</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>general</t>
+          <t>caballeros</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Núñez, Valentino</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>41</v>
+          <t>Malvasio, Joaquín</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>NPT</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -704,6 +747,11 @@
       <c r="F10" t="n">
         <v>93</v>
       </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -732,6 +780,11 @@
       <c r="F11" t="n">
         <v>79</v>
       </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -760,6 +813,11 @@
       <c r="F12" t="n">
         <v>93</v>
       </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -788,6 +846,11 @@
       <c r="F13" t="n">
         <v>86</v>
       </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -816,6 +879,11 @@
       <c r="F14" t="n">
         <v>75</v>
       </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -843,6 +911,11 @@
       </c>
       <c r="F15" t="n">
         <v>82</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update resultados - 2026-02-25 22:02:07
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -461,12 +461,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>####1er Torneo Federativo - C.A.E. - Juveniles, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
+          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Eagles</t>
+          <t>Prejuveniles</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -479,11 +479,11 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>De Bueno, Benjamín</t>
+          <t>Garrone, Federico Daniel</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update resultados - 2026-02-25 22:03:52
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -466,7 +466,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Prejuveniles</t>
+          <t>Eagles</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -479,11 +479,11 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Garrone, Federico Daniel</t>
+          <t>Saure, Pedro Adolfo</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update resultados - 2026-02-25 22:06:48
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,6 +491,39 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Prejuveniles</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>caballeros</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Petric, Juan Cruz</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>82</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update resultados - 2026-02-26 00:16:14
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -512,11 +512,11 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Petric, Juan Cruz</t>
+          <t>Luján Martínez, Benjamín</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update resultados - 2026-02-26 00:18:24
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,11 +452,6 @@
           <t>total</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>estado</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -485,11 +480,6 @@
       <c r="F2" t="n">
         <v>49</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -518,10 +508,33 @@
       <c r="F3" t="n">
         <v>75</v>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>OK</t>
-        </is>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Prejuveniles</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>caballeros</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Petric, Juan Cruz</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update resultados - 2026-02-26 00:53:21
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,16 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>dia_1</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>dia_2</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
           <t>total</t>
         </is>
       </c>
@@ -480,6 +490,10 @@
       <c r="F2" t="n">
         <v>49</v>
       </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="n">
+        <v>49</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -489,7 +503,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Prejuveniles</t>
+          <t>Albatros</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -506,7 +520,11 @@
         </is>
       </c>
       <c r="F3" t="n">
-        <v>75</v>
+        <v>84</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="n">
+        <v>84</v>
       </c>
     </row>
     <row r="4">
@@ -526,15 +544,55 @@
         </is>
       </c>
       <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Luján Martínez, Benjamín</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>75</v>
+      </c>
+      <c r="G4" t="n">
+        <v>84</v>
+      </c>
+      <c r="H4" t="n">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Prejuveniles</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>caballeros</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
         <v>2</v>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Petric, Juan Cruz</t>
         </is>
       </c>
-      <c r="F4" t="n">
+      <c r="F5" t="n">
         <v>81</v>
+      </c>
+      <c r="G5" t="n">
+        <v>79</v>
+      </c>
+      <c r="H5" t="n">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update resultados - 2026-02-28 15:32:28
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -548,17 +548,15 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Luján Martínez, Benjamín</t>
+          <t>Kern Pascuali, Juan Daniel</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>75</v>
-      </c>
-      <c r="G4" t="n">
-        <v>84</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
-        <v>159</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5">
@@ -582,16 +580,50 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
+          <t>Luján Martínez, Benjamín</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>75</v>
+      </c>
+      <c r="G5" t="n">
+        <v>84</v>
+      </c>
+      <c r="H5" t="n">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Prejuveniles</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>caballeros</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>Petric, Juan Cruz</t>
         </is>
       </c>
-      <c r="F5" t="n">
+      <c r="F6" t="n">
         <v>81</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G6" t="n">
         <v>79</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H6" t="n">
         <v>160</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update resultados - 2026-02-28 15:38:01
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,7 +471,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Eagles</t>
+          <t>Prejuveniles</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -484,15 +484,15 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Saure, Pedro Adolfo</t>
+          <t>Kern Pascuali, Juan Daniel</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
-        <v>49</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3">
@@ -503,7 +503,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Albatros</t>
+          <t>Prejuveniles</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -520,111 +520,13 @@
         </is>
       </c>
       <c r="F3" t="n">
+        <v>75</v>
+      </c>
+      <c r="G3" t="n">
         <v>84</v>
       </c>
-      <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Prejuveniles</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>caballeros</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Kern Pascuali, Juan Daniel</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>92</v>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Prejuveniles</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>caballeros</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Luján Martínez, Benjamín</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>75</v>
-      </c>
-      <c r="G5" t="n">
-        <v>84</v>
-      </c>
-      <c r="H5" t="n">
         <v>159</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Prejuveniles</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>caballeros</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>3</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Petric, Juan Cruz</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>81</v>
-      </c>
-      <c r="G6" t="n">
-        <v>79</v>
-      </c>
-      <c r="H6" t="n">
-        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update resultados - 2026-02-28 15:44:22
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,40 +495,6 @@
         <v>92</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Prejuveniles</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>caballeros</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>2</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Luján Martínez, Benjamín</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>75</v>
-      </c>
-      <c r="G3" t="n">
-        <v>84</v>
-      </c>
-      <c r="H3" t="n">
-        <v>159</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update resultados - 2026-02-28 15:47:20
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,12 +471,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Prejuveniles</t>
+          <t>Albatros</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>caballeros</t>
+          <t>damas</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -484,14 +484,78 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Kern Pascuali, Juan Daniel</t>
+          <t>Ferrante Keller, María Estefanía</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Prejuveniles</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>damas</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Ferrante Keller, María Estefanía</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="n">
+        <v>115</v>
+      </c>
+      <c r="H3" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Prejuveniles</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>caballeros</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Kern Pascuali, Juan Daniel</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>92</v>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="n">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update resultados - 2026-02-28 15:50:41
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,7 +471,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Albatros</t>
+          <t>Prejuveniles</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -487,10 +487,10 @@
           <t>Ferrante Keller, María Estefanía</t>
         </is>
       </c>
-      <c r="F2" t="n">
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="n">
         <v>115</v>
       </c>
-      <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
         <v>115</v>
       </c>
@@ -508,7 +508,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>damas</t>
+          <t>caballeros</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -516,46 +516,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Ferrante Keller, María Estefanía</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="n">
-        <v>115</v>
-      </c>
+          <t>Kern Pascuali, Juan Daniel</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>92</v>
+      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Prejuveniles</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>caballeros</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Kern Pascuali, Juan Daniel</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>92</v>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update resultados - 2026-02-28 15:52:25
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -487,10 +487,10 @@
           <t>Ferrante Keller, María Estefanía</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="n">
+      <c r="F2" t="n">
         <v>115</v>
       </c>
+      <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
         <v>115</v>
       </c>

</xml_diff>

<commit_message>
Update resultados - 2026-02-28 16:17:23
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -527,6 +527,38 @@
         <v>92</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Juveniles</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>caballeros</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Liberatori, Augusto</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>83</v>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="n">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update resultados - 2026-02-28 16:18:37
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -559,6 +559,38 @@
         <v>83</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Juveniles</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>damas</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Martínez, Valentina</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>84</v>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="n">
+        <v>84</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update resultados - 2026-02-28 16:20:07
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -591,6 +591,38 @@
         <v>84</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Sub23</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>caballeros</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Minigutti, Ignacio</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>100</v>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="n">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update resultados - 2026-02-28 16:35:27
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,12 +471,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Prejuveniles</t>
+          <t>Albatros</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>damas</t>
+          <t>caballeros</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -484,15 +484,15 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Ferrante Keller, María Estefanía</t>
+          <t>Luján Martínez, Benjamín</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
-        <v>115</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3">
@@ -508,7 +508,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>caballeros</t>
+          <t>damas</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -516,15 +516,15 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Kern Pascuali, Juan Daniel</t>
+          <t>Ferrante Keller, María Estefanía</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>92</v>
+        <v>115</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
-        <v>92</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4">
@@ -535,7 +535,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Juveniles</t>
+          <t>Prejuveniles</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -548,15 +548,15 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Liberatori, Augusto</t>
+          <t>Kern Pascuali, Juan Daniel</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
-        <v>83</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5">
@@ -567,28 +567,28 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Juveniles</t>
+          <t>Prejuveniles</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>damas</t>
+          <t>caballeros</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Martínez, Valentina</t>
-        </is>
-      </c>
-      <c r="F5" t="n">
-        <v>84</v>
-      </c>
-      <c r="G5" t="inlineStr"/>
+          <t>Luján Martínez, Benjamín</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="n">
+        <v>98</v>
+      </c>
       <c r="H5" t="n">
-        <v>84</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6">
@@ -599,7 +599,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sub23</t>
+          <t>Juveniles</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -612,14 +612,78 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Minigutti, Ignacio</t>
+          <t>Liberatori, Augusto</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Juveniles</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>damas</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Martínez, Valentina</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>84</v>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Sub23</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>caballeros</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Minigutti, Ignacio</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>100</v>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update resultados - 2026-02-28 16:36:43
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -471,12 +471,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Albatros</t>
+          <t>Prejuveniles</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>caballeros</t>
+          <t>damas</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -484,15 +484,15 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Luján Martínez, Benjamín</t>
+          <t>Ferrante Keller, María Estefanía</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="n">
-        <v>98</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3">
@@ -508,7 +508,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>damas</t>
+          <t>caballeros</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -516,15 +516,15 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Ferrante Keller, María Estefanía</t>
+          <t>Kern Pascuali, Juan Daniel</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
-        <v>115</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4">
@@ -544,19 +544,19 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Kern Pascuali, Juan Daniel</t>
-        </is>
-      </c>
-      <c r="F4" t="n">
-        <v>92</v>
-      </c>
-      <c r="G4" t="inlineStr"/>
+          <t>Luján Martínez, Benjamín</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="n">
+        <v>98</v>
+      </c>
       <c r="H4" t="n">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5">
@@ -567,7 +567,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Prejuveniles</t>
+          <t>Juveniles</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -576,19 +576,19 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Luján Martínez, Benjamín</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="n">
-        <v>98</v>
-      </c>
+          <t>Liberatori, Augusto</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>83</v>
+      </c>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
-        <v>98</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6">
@@ -604,7 +604,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>caballeros</t>
+          <t>damas</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -612,15 +612,15 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Liberatori, Augusto</t>
+          <t>Martínez, Valentina</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7">
@@ -631,12 +631,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Juveniles</t>
+          <t>Sub23</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>damas</t>
+          <t>caballeros</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -644,46 +644,14 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Martínez, Valentina</t>
+          <t>Minigutti, Ignacio</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Sub23</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>caballeros</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Minigutti, Ignacio</t>
-        </is>
-      </c>
-      <c r="F8" t="n">
-        <v>100</v>
-      </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update resultados - 2026-02-28 16:37:58
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -551,10 +551,10 @@
           <t>Luján Martínez, Benjamín</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="n">
+      <c r="F4" t="n">
         <v>98</v>
       </c>
+      <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
Update resultados - 2026-02-28 16:39:53
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -604,23 +604,23 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>damas</t>
+          <t>caballeros</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Martínez, Valentina</t>
+          <t>Vega, Ramón Emanuel</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7">
@@ -631,12 +631,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Sub23</t>
+          <t>Juveniles</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>caballeros</t>
+          <t>damas</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -644,14 +644,46 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Minigutti, Ignacio</t>
+          <t>Martínez, Valentina</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Sub23</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>caballeros</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Minigutti, Ignacio</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>100</v>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update resultados - 2026-02-28 16:42:38
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -676,14 +676,46 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Minigutti, Ignacio</t>
+          <t>Rodriguez, Santiago</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Sub23</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>caballeros</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Minigutti, Ignacio</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>100</v>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update resultados - 2026-02-28 16:43:39
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -567,7 +567,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Juveniles</t>
+          <t>Prejuveniles</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -576,19 +576,19 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Liberatori, Augusto</t>
+          <t>Garrone, Federico Daniel</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
-        <v>83</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6">
@@ -608,19 +608,19 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Vega, Ramón Emanuel</t>
+          <t>Liberatori, Augusto</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7">
@@ -636,23 +636,23 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>damas</t>
+          <t>caballeros</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Martínez, Valentina</t>
+          <t>Vega, Ramón Emanuel</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8">
@@ -663,12 +663,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Sub23</t>
+          <t>Juveniles</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>caballeros</t>
+          <t>damas</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -676,15 +676,15 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Rodriguez, Santiago</t>
+          <t>Martínez, Valentina</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9">
@@ -704,18 +704,50 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Minigutti, Ignacio</t>
+          <t>Rodriguez, Santiago</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Sub23</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>caballeros</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Minigutti, Ignacio</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>100</v>
+      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update resultados - 2026-02-28 16:47:58
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,15 +516,15 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Kern Pascuali, Juan Daniel</t>
+          <t>Petric, Juan Cruz</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="n">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4">
@@ -548,15 +548,15 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Luján Martínez, Benjamín</t>
+          <t>Kern Pascuali, Juan Daniel</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="n">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5">
@@ -580,15 +580,15 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Garrone, Federico Daniel</t>
+          <t>Luján Martínez, Benjamín</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="n">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6">
@@ -599,7 +599,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Juveniles</t>
+          <t>Prejuveniles</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -608,19 +608,19 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Liberatori, Augusto</t>
+          <t>Garrone, Federico Daniel</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="n">
-        <v>83</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7">
@@ -640,19 +640,19 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Vega, Ramón Emanuel</t>
+          <t>Liberatori, Augusto</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8">
@@ -668,23 +668,23 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>damas</t>
+          <t>caballeros</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Martínez, Valentina</t>
+          <t>Vega, Ramón Emanuel</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9">
@@ -695,12 +695,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Sub23</t>
+          <t>Juveniles</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>caballeros</t>
+          <t>damas</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -708,15 +708,15 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Rodriguez, Santiago</t>
+          <t>Martínez, Valentina</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10">
@@ -736,18 +736,82 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Minigutti, Ignacio</t>
+          <t>Suárez, Fermín Irú</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Sub23</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>caballeros</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Rodriguez, Santiago</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>83</v>
+      </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Sub23</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>caballeros</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>3</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Minigutti, Ignacio</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>100</v>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update resultados - 2026-02-28 16:49:12
</commit_message>
<xml_diff>
--- a/docs/resultados.xlsx
+++ b/docs/resultados.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -700,23 +700,23 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>damas</t>
+          <t>caballeros</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Martínez, Valentina</t>
+          <t>Cejas, Pedro Gonzalo</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="n">
-        <v>84</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10">
@@ -727,12 +727,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Sub23</t>
+          <t>Juveniles</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>caballeros</t>
+          <t>damas</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -740,15 +740,15 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Suárez, Fermín Irú</t>
+          <t>Martínez, Valentina</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="n">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11">
@@ -768,19 +768,19 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Rodriguez, Santiago</t>
+          <t>Suárez, Fermín Irú</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="n">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12">
@@ -800,18 +800,50 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Minigutti, Ignacio</t>
+          <t>Rodriguez, Santiago</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>####1er Torneo Federativo - C.A.E. - Sub 23, Prejuveniles y sub 23 (28 de Febrero y 1 de Marzo) - Juniors (Domingo 1 de Marzo)</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Sub23</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>caballeros</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>3</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Minigutti, Ignacio</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>100</v>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>